<commit_message>
update the excel of exam massages
</commit_message>
<xml_diff>
--- a/guide/UniversityForm.xlsx
+++ b/guide/UniversityForm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="4428" windowHeight="2928"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="4425" windowHeight="2925"/>
   </bookViews>
   <sheets>
     <sheet name="备选学校分析" sheetId="1" r:id="rId1"/>
@@ -15,11 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="166">
-  <si>
-    <t>序号</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="167">
   <si>
     <t>学校</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -46,10 +42,6 @@
   </si>
   <si>
     <t>复试科目</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>拟招生人数</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -518,10 +510,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>中国农业大学</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>海淀西土城路</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -570,10 +558,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>共1.2*6=7.2w</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>海淀区清华东路</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -613,10 +597,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>北京理工大学</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>海淀区学院路</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -632,14 +612,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>电子信息</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>3年</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>549 计算机综合二（含系统结构、操作系统、软件工程）</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -657,10 +629,6 @@
   </si>
   <si>
     <t>信息学院</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>电子信息</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -681,10 +649,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>2年</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>http://gs.cufe.edu.cn/zsgz/sszs_sz_.htm</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -698,6 +662,46 @@
   </si>
   <si>
     <t>共0.6w*3=1.8w</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>共1.2*3=7.2w</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>学校信息</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>专业信息</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>共1.2*3=7.2w</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>拟招生人数（不含推免）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>报名人数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>录取人数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>报录比</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>分数线</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -745,7 +749,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -762,8 +766,32 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -771,6 +799,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -782,7 +862,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -793,11 +873,84 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1107,376 +1260,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+      <selection pane="topRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="1" customWidth="1"/>
-    <col min="3" max="5" width="28.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.109375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="6.75" style="13" customWidth="1"/>
+    <col min="2" max="2" width="8.875" style="13"/>
+    <col min="3" max="5" width="8.875" style="15"/>
+    <col min="6" max="6" width="17.25" style="15" customWidth="1"/>
+    <col min="7" max="7" width="17" style="15" customWidth="1"/>
+    <col min="8" max="11" width="8.875" style="19"/>
+    <col min="12" max="15" width="8.875" style="28"/>
+    <col min="16" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:18" s="13" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+    </row>
+    <row r="2" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1">
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1">
+      <c r="E2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1">
+      <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1">
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="H2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="81" x14ac:dyDescent="0.15">
+      <c r="A3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="18">
+        <v>21</v>
+      </c>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18">
+        <v>10</v>
+      </c>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="Q3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="D4" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4" s="18">
+        <v>155</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18">
+        <v>6</v>
+      </c>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="18">
+        <v>38</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18">
+        <v>5</v>
+      </c>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="R5" s="5"/>
+    </row>
+    <row r="6" spans="1:18" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="18">
+        <v>74</v>
+      </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q6" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="R6" s="5"/>
+    </row>
+    <row r="7" spans="1:18" ht="148.5" x14ac:dyDescent="0.15">
+      <c r="A7" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="18">
+        <v>41</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A8" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="H8" s="18">
+        <v>33</v>
+      </c>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18">
+        <v>8.9</v>
+      </c>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="R8" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="I2" s="1" t="s">
+    </row>
+    <row r="9" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+      <c r="A9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+    </row>
+    <row r="10" spans="1:18" ht="81" x14ac:dyDescent="0.15">
+      <c r="A10" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" s="18">
+        <v>8</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="27">
+        <v>356</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q10" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="86.4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="100.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1">
-        <v>155</v>
-      </c>
-      <c r="D9" s="1">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1">
-        <v>74</v>
-      </c>
-      <c r="F9" s="1">
-        <v>41</v>
-      </c>
-      <c r="G9" s="1">
-        <v>33</v>
-      </c>
-      <c r="I9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="1">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1">
-        <v>5</v>
-      </c>
-      <c r="G14" s="1">
-        <v>8.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="72" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="R10" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>162</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="D4:D6"/>
+  </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1"/>
-    <hyperlink ref="C17" r:id="rId2"/>
-    <hyperlink ref="F17" r:id="rId3"/>
-    <hyperlink ref="G17" r:id="rId4"/>
-    <hyperlink ref="I17" r:id="rId5"/>
+    <hyperlink ref="R3" r:id="rId1"/>
+    <hyperlink ref="R4" r:id="rId2"/>
+    <hyperlink ref="R7" r:id="rId3"/>
+    <hyperlink ref="R8" r:id="rId4"/>
+    <hyperlink ref="R10" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -1491,370 +1698,370 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.375" style="1" customWidth="1"/>
+    <col min="2" max="3" width="19.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.75" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I2" s="2">
         <v>985</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I3" s="3">
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="1" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="1" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="1" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D14" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D16" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+    <row r="17" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="1" t="s">
+    <row r="18" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
+    <row r="19" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
+    <row r="20" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="s">
+    <row r="21" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="1" t="s">
+    <row r="22" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="1" t="s">
+    <row r="23" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D23" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="1" t="s">
+    <row r="24" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D24" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="1" t="s">
+    <row r="25" spans="4:6" x14ac:dyDescent="0.15">
+      <c r="D25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>